<commit_message>
dispersal modified and seemingly working
</commit_message>
<xml_diff>
--- a/inst/extdata/rotations-paper-inputs-201910.xlsx
+++ b/inst/extdata/rotations-paper-inputs-201910.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rsprojects\rotations\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC059EBD-22BE-47AB-83ED-ADA98963B69A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFC8EAE-C146-424C-BD9C-6D9915DA9F59}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="255" yWindow="195" windowWidth="28320" windowHeight="13830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="expt_rot_mort_dispersal" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
   <si>
     <t xml:space="preserve"> BEWARE that if add a row here also need to add to set_run_inputs.r </t>
   </si>
@@ -155,9 +155,6 @@
   </si>
   <si>
     <t>A4-freq-insame-costs-disp</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> :</t>
   </si>
   <si>
     <t>infile-see-rotation_runs2019.Rmd</t>
@@ -1013,30 +1010,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q37"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="20" topLeftCell="G21" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="32.06640625" customWidth="1"/>
-    <col min="2" max="2" width="32.59765625" customWidth="1"/>
-    <col min="3" max="4" width="28.265625" customWidth="1"/>
-    <col min="5" max="5" width="29.73046875" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.1328125" customWidth="1"/>
+    <col min="4" max="4" width="24.9296875" customWidth="1"/>
+    <col min="5" max="5" width="22.3984375" customWidth="1"/>
     <col min="6" max="6" width="26.796875" customWidth="1"/>
-    <col min="7" max="8" width="28.265625" customWidth="1"/>
-    <col min="9" max="9" width="29.73046875" customWidth="1"/>
+    <col min="7" max="7" width="24.53125" customWidth="1"/>
+    <col min="8" max="8" width="25.19921875" customWidth="1"/>
+    <col min="9" max="9" width="24.9296875" customWidth="1"/>
     <col min="10" max="11" width="18.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
         <v>42</v>
@@ -1051,16 +1048,16 @@
         <v>44</v>
       </c>
       <c r="F1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" t="s">
         <v>47</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>48</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>49</v>
-      </c>
-      <c r="I1" t="s">
-        <v>50</v>
       </c>
       <c r="J1" t="s">
         <v>39</v>
@@ -1068,11 +1065,11 @@
       <c r="K1" t="s">
         <v>40</v>
       </c>
-      <c r="Q1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="L1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1082,6 +1079,9 @@
       <c r="C2">
         <v>1</v>
       </c>
+      <c r="D2">
+        <v>0.1</v>
+      </c>
       <c r="E2">
         <v>0.1</v>
       </c>
@@ -1091,6 +1091,9 @@
       <c r="G2">
         <v>1</v>
       </c>
+      <c r="H2">
+        <v>0.1</v>
+      </c>
       <c r="I2">
         <v>0.1</v>
       </c>
@@ -1101,7 +1104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1111,6 +1114,9 @@
       <c r="C3">
         <v>1</v>
       </c>
+      <c r="D3">
+        <v>0.9</v>
+      </c>
       <c r="E3">
         <v>0.9</v>
       </c>
@@ -1120,6 +1126,9 @@
       <c r="G3">
         <v>1</v>
       </c>
+      <c r="H3">
+        <v>0.9</v>
+      </c>
       <c r="I3">
         <v>0.9</v>
       </c>
@@ -1130,7 +1139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1140,17 +1149,23 @@
       <c r="C4">
         <v>0</v>
       </c>
+      <c r="D4">
+        <v>0.01</v>
+      </c>
       <c r="E4">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
+      <c r="H4">
+        <v>0.01</v>
+      </c>
       <c r="I4">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -1159,7 +1174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1169,17 +1184,23 @@
       <c r="C5">
         <v>0</v>
       </c>
+      <c r="D5">
+        <v>0.3</v>
+      </c>
       <c r="E5">
-        <v>0.9</v>
+        <v>0.3</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
+      <c r="H5">
+        <v>0.3</v>
+      </c>
       <c r="I5">
-        <v>0.9</v>
+        <v>0.3</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -1188,7 +1209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1198,6 +1219,9 @@
       <c r="C6">
         <v>500</v>
       </c>
+      <c r="D6">
+        <v>500</v>
+      </c>
       <c r="E6">
         <v>500</v>
       </c>
@@ -1207,6 +1231,9 @@
       <c r="G6">
         <v>500</v>
       </c>
+      <c r="H6">
+        <v>500</v>
+      </c>
       <c r="I6">
         <v>500</v>
       </c>
@@ -1217,7 +1244,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1227,6 +1254,9 @@
       <c r="C7">
         <v>10</v>
       </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
       <c r="E7">
         <v>10</v>
       </c>
@@ -1236,6 +1266,9 @@
       <c r="G7">
         <v>10</v>
       </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
       <c r="I7">
         <v>10</v>
       </c>
@@ -1246,7 +1279,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1256,6 +1289,9 @@
       <c r="C8">
         <v>10</v>
       </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
       <c r="E8">
         <v>10</v>
       </c>
@@ -1265,6 +1301,9 @@
       <c r="G8">
         <v>10</v>
       </c>
+      <c r="H8">
+        <v>10</v>
+      </c>
       <c r="I8">
         <v>10</v>
       </c>
@@ -1275,7 +1314,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1285,6 +1324,9 @@
       <c r="C9">
         <v>0</v>
       </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
       <c r="E9">
         <v>0</v>
       </c>
@@ -1294,6 +1336,9 @@
       <c r="G9">
         <v>0</v>
       </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
       <c r="I9">
         <v>0</v>
       </c>
@@ -1304,7 +1349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1314,6 +1359,9 @@
       <c r="C10">
         <v>0</v>
       </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
       <c r="E10">
         <v>0</v>
       </c>
@@ -1323,6 +1371,9 @@
       <c r="G10">
         <v>0</v>
       </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
       <c r="I10">
         <v>0</v>
       </c>
@@ -1333,7 +1384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1343,6 +1394,9 @@
       <c r="C11">
         <v>0</v>
       </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
       <c r="E11">
         <v>0</v>
       </c>
@@ -1352,6 +1406,9 @@
       <c r="G11">
         <v>0</v>
       </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
       <c r="I11">
         <v>0</v>
       </c>
@@ -1362,7 +1419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1372,6 +1429,9 @@
       <c r="C12" t="s">
         <v>38</v>
       </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
       <c r="E12" t="s">
         <v>38</v>
       </c>
@@ -1381,6 +1441,9 @@
       <c r="G12" t="s">
         <v>38</v>
       </c>
+      <c r="H12" t="s">
+        <v>38</v>
+      </c>
       <c r="I12" t="s">
         <v>38</v>
       </c>
@@ -1391,7 +1454,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1401,6 +1464,9 @@
       <c r="C13">
         <v>0.9</v>
       </c>
+      <c r="D13">
+        <v>0.9</v>
+      </c>
       <c r="E13">
         <v>0.9</v>
       </c>
@@ -1410,6 +1476,9 @@
       <c r="G13">
         <v>0.9</v>
       </c>
+      <c r="H13">
+        <v>0.9</v>
+      </c>
       <c r="I13">
         <v>0.9</v>
       </c>
@@ -1420,7 +1489,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1430,6 +1499,9 @@
       <c r="C14">
         <v>0.5</v>
       </c>
+      <c r="D14">
+        <v>0.5</v>
+      </c>
       <c r="E14">
         <v>0.5</v>
       </c>
@@ -1439,6 +1511,9 @@
       <c r="G14">
         <v>0.5</v>
       </c>
+      <c r="H14">
+        <v>0.5</v>
+      </c>
       <c r="I14">
         <v>0.5</v>
       </c>
@@ -1449,7 +1524,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1459,8 +1534,11 @@
       <c r="C15">
         <v>1</v>
       </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
       <c r="E15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -1468,8 +1546,11 @@
       <c r="G15">
         <v>1</v>
       </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
       <c r="I15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15">
         <v>1</v>
@@ -1478,7 +1559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1488,6 +1569,9 @@
       <c r="C16">
         <v>0</v>
       </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
       <c r="E16">
         <v>0</v>
       </c>
@@ -1495,6 +1579,9 @@
         <v>0</v>
       </c>
       <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
@@ -1517,14 +1604,20 @@
       <c r="C17">
         <v>0.1</v>
       </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
       <c r="E17">
         <v>0.1</v>
       </c>
       <c r="F17">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G17">
         <v>0.1</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
       </c>
       <c r="I17">
         <v>0.1</v>
@@ -1546,6 +1639,9 @@
       <c r="C18">
         <v>0.4</v>
       </c>
+      <c r="D18">
+        <v>0.4</v>
+      </c>
       <c r="E18">
         <v>0.4</v>
       </c>
@@ -1553,6 +1649,9 @@
         <v>0.4</v>
       </c>
       <c r="G18">
+        <v>0.4</v>
+      </c>
+      <c r="H18">
         <v>0.4</v>
       </c>
       <c r="I18">
@@ -1575,6 +1674,9 @@
       <c r="C19">
         <v>0.9</v>
       </c>
+      <c r="D19">
+        <v>0.9</v>
+      </c>
       <c r="E19">
         <v>0.9</v>
       </c>
@@ -1582,6 +1684,9 @@
         <v>0.9</v>
       </c>
       <c r="G19">
+        <v>0.9</v>
+      </c>
+      <c r="H19">
         <v>0.9</v>
       </c>
       <c r="I19">
@@ -1599,22 +1704,28 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
       </c>
       <c r="I20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20">
         <v>1</v>
@@ -1633,6 +1744,9 @@
       <c r="C21">
         <v>1</v>
       </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
       <c r="E21">
         <v>1</v>
       </c>
@@ -1640,6 +1754,9 @@
         <v>1</v>
       </c>
       <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
         <v>1</v>
       </c>
       <c r="I21">
@@ -1662,13 +1779,19 @@
       <c r="C22">
         <v>0.7</v>
       </c>
+      <c r="D22">
+        <v>0.7</v>
+      </c>
       <c r="E22">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="F22">
         <v>0.7</v>
       </c>
       <c r="G22">
+        <v>0.7</v>
+      </c>
+      <c r="H22">
         <v>0.7</v>
       </c>
       <c r="I22">
@@ -1691,6 +1814,9 @@
       <c r="C23">
         <v>1</v>
       </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
       <c r="E23">
         <v>1</v>
       </c>
@@ -1698,6 +1824,9 @@
         <v>1</v>
       </c>
       <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
         <v>1</v>
       </c>
       <c r="I23">
@@ -1720,6 +1849,9 @@
       <c r="C24">
         <v>0.1</v>
       </c>
+      <c r="D24">
+        <v>0.1</v>
+      </c>
       <c r="E24">
         <v>0.1</v>
       </c>
@@ -1727,6 +1859,9 @@
         <v>0.1</v>
       </c>
       <c r="G24">
+        <v>0.1</v>
+      </c>
+      <c r="H24">
         <v>0.1</v>
       </c>
       <c r="I24">
@@ -1749,6 +1884,9 @@
       <c r="C25">
         <v>0.9</v>
       </c>
+      <c r="D25">
+        <v>0.9</v>
+      </c>
       <c r="E25">
         <v>0.9</v>
       </c>
@@ -1756,6 +1894,9 @@
         <v>0.9</v>
       </c>
       <c r="G25">
+        <v>0.9</v>
+      </c>
+      <c r="H25">
         <v>0.9</v>
       </c>
       <c r="I25">
@@ -1778,6 +1919,9 @@
       <c r="C26">
         <v>0</v>
       </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
       <c r="E26">
         <v>0</v>
       </c>
@@ -1785,6 +1929,9 @@
         <v>0</v>
       </c>
       <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
         <v>0</v>
       </c>
       <c r="I26">
@@ -1807,6 +1954,9 @@
       <c r="C27">
         <v>1</v>
       </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
       <c r="E27">
         <v>1</v>
       </c>
@@ -1814,6 +1964,9 @@
         <v>1</v>
       </c>
       <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
         <v>1</v>
       </c>
       <c r="I27">
@@ -1836,6 +1989,9 @@
       <c r="C28">
         <v>0</v>
       </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
       <c r="E28">
         <v>0</v>
       </c>
@@ -1843,6 +1999,9 @@
         <v>0</v>
       </c>
       <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
         <v>0</v>
       </c>
       <c r="I28">
@@ -1865,6 +2024,9 @@
       <c r="C29">
         <v>1</v>
       </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
       <c r="E29">
         <v>1</v>
       </c>
@@ -1872,6 +2034,9 @@
         <v>1</v>
       </c>
       <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
         <v>1</v>
       </c>
       <c r="I29">
@@ -1894,13 +2059,19 @@
       <c r="C30">
         <v>1E-3</v>
       </c>
+      <c r="D30">
+        <v>1E-3</v>
+      </c>
       <c r="E30">
         <v>1E-3</v>
       </c>
       <c r="F30">
-        <v>5.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="G30">
+        <v>1E-3</v>
+      </c>
+      <c r="H30">
         <v>1E-3</v>
       </c>
       <c r="I30">
@@ -1923,6 +2094,9 @@
       <c r="C31">
         <v>0.1</v>
       </c>
+      <c r="D31">
+        <v>0.1</v>
+      </c>
       <c r="E31">
         <v>0.1</v>
       </c>
@@ -1930,6 +2104,9 @@
         <v>0.1</v>
       </c>
       <c r="G31">
+        <v>0.1</v>
+      </c>
+      <c r="H31">
         <v>0.1</v>
       </c>
       <c r="I31">
@@ -1952,8 +2129,11 @@
       <c r="C32">
         <v>2</v>
       </c>
-      <c r="E32" t="s">
-        <v>45</v>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
       </c>
       <c r="F32">
         <v>2</v>
@@ -1961,8 +2141,11 @@
       <c r="G32">
         <v>2</v>
       </c>
-      <c r="I32" t="s">
-        <v>45</v>
+      <c r="H32">
+        <v>2</v>
+      </c>
+      <c r="I32">
+        <v>2</v>
       </c>
       <c r="J32">
         <v>2</v>
@@ -1981,6 +2164,9 @@
       <c r="C33">
         <v>5</v>
       </c>
+      <c r="D33">
+        <v>5</v>
+      </c>
       <c r="E33">
         <v>5</v>
       </c>
@@ -1988,6 +2174,9 @@
         <v>5</v>
       </c>
       <c r="G33">
+        <v>5</v>
+      </c>
+      <c r="H33">
         <v>5</v>
       </c>
       <c r="I33">
@@ -2010,6 +2199,9 @@
       <c r="C34">
         <v>10</v>
       </c>
+      <c r="D34">
+        <v>10</v>
+      </c>
       <c r="E34">
         <v>10</v>
       </c>
@@ -2017,6 +2209,9 @@
         <v>10</v>
       </c>
       <c r="G34">
+        <v>10</v>
+      </c>
+      <c r="H34">
         <v>10</v>
       </c>
       <c r="I34">
@@ -2039,6 +2234,9 @@
       <c r="C35">
         <v>10</v>
       </c>
+      <c r="D35">
+        <v>10</v>
+      </c>
       <c r="E35">
         <v>10</v>
       </c>
@@ -2046,6 +2244,9 @@
         <v>20</v>
       </c>
       <c r="G35">
+        <v>10</v>
+      </c>
+      <c r="H35">
         <v>10</v>
       </c>
       <c r="I35">
@@ -2068,6 +2269,9 @@
       <c r="C36">
         <v>0</v>
       </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
       <c r="E36">
         <v>0</v>
       </c>
@@ -2100,6 +2304,9 @@
       <c r="C37">
         <v>2</v>
       </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
       <c r="E37">
         <v>2</v>
       </c>
@@ -2107,6 +2314,9 @@
         <v>2</v>
       </c>
       <c r="G37">
+        <v>2</v>
+      </c>
+      <c r="H37">
         <v>2</v>
       </c>
       <c r="I37">

</xml_diff>

<commit_message>
runs now mostly working for expts C and D
</commit_message>
<xml_diff>
--- a/inst/extdata/rotations-paper-inputs-201910.xlsx
+++ b/inst/extdata/rotations-paper-inputs-201910.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rsprojects\rotations\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFC8EAE-C146-424C-BD9C-6D9915DA9F59}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D91A77A-2352-421C-9503-D2C7F338966D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="255" yWindow="195" windowWidth="28320" windowHeight="13830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="expt_rot_mort_dispersal" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
   <si>
     <t xml:space="preserve"> BEWARE that if add a row here also need to add to set_run_inputs.r </t>
   </si>
@@ -139,12 +139,6 @@
     <t>freq</t>
   </si>
   <si>
-    <t>C mort insame</t>
-  </si>
-  <si>
-    <t>D mort insdif</t>
-  </si>
-  <si>
     <t>A2-freq-insame-costs-nodisp</t>
   </si>
   <si>
@@ -170,6 +164,30 @@
   </si>
   <si>
     <t>B4-freq-insdiff-costs-disp</t>
+  </si>
+  <si>
+    <t>C1-mort-insame-nocosts-nodisp</t>
+  </si>
+  <si>
+    <t>C2-mort-insame-costs-nodisp</t>
+  </si>
+  <si>
+    <t>C3-mort-insame-nocosts-disp</t>
+  </si>
+  <si>
+    <t>C4-mort-insame-costs-disp</t>
+  </si>
+  <si>
+    <t>D3-mort-insdiff-nocosts-disp</t>
+  </si>
+  <si>
+    <t>D4-mort-insdiff-costs-disp</t>
+  </si>
+  <si>
+    <t>D2-mort-insdiff-costs-nodisp</t>
+  </si>
+  <si>
+    <t>D1-mort-insdiff-nocosts-nodisp</t>
   </si>
 </sst>
 </file>
@@ -1010,66 +1028,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N36" sqref="N36:Q36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.06640625" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
-    <col min="3" max="3" width="24.1328125" customWidth="1"/>
-    <col min="4" max="4" width="24.9296875" customWidth="1"/>
-    <col min="5" max="5" width="22.3984375" customWidth="1"/>
-    <col min="6" max="6" width="26.796875" customWidth="1"/>
-    <col min="7" max="7" width="24.53125" customWidth="1"/>
-    <col min="8" max="8" width="25.19921875" customWidth="1"/>
-    <col min="9" max="9" width="24.9296875" customWidth="1"/>
-    <col min="10" max="11" width="18.1328125" customWidth="1"/>
+    <col min="1" max="1" width="32" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" customWidth="1"/>
+    <col min="8" max="8" width="25.140625" customWidth="1"/>
+    <col min="9" max="9" width="25" customWidth="1"/>
+    <col min="10" max="10" width="26.28515625" customWidth="1"/>
+    <col min="11" max="11" width="24.140625" customWidth="1"/>
+    <col min="12" max="12" width="25" customWidth="1"/>
+    <col min="13" max="13" width="22.42578125" customWidth="1"/>
+    <col min="14" max="14" width="26.28515625" customWidth="1"/>
+    <col min="15" max="15" width="24.140625" customWidth="1"/>
+    <col min="16" max="16" width="25" customWidth="1"/>
+    <col min="17" max="17" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>46</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>47</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>48</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>49</v>
       </c>
-      <c r="J1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K1" t="s">
-        <v>40</v>
-      </c>
       <c r="L1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+        <v>50</v>
+      </c>
+      <c r="M1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" t="s">
+        <v>54</v>
+      </c>
+      <c r="P1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1103,8 +1146,26 @@
       <c r="K2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L2">
+        <v>0.1</v>
+      </c>
+      <c r="M2">
+        <v>0.1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>0.1</v>
+      </c>
+      <c r="Q2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1138,8 +1199,26 @@
       <c r="K3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L3">
+        <v>0.9</v>
+      </c>
+      <c r="M3">
+        <v>0.9</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>0.9</v>
+      </c>
+      <c r="Q3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1168,13 +1247,31 @@
         <v>0.01</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0.01</v>
+      </c>
+      <c r="M4">
+        <v>0.01</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0.01</v>
+      </c>
+      <c r="Q4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1203,13 +1300,31 @@
         <v>0.3</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0.3</v>
+      </c>
+      <c r="M5">
+        <v>0.3</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0.3</v>
+      </c>
+      <c r="Q5">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1243,8 +1358,26 @@
       <c r="K6">
         <v>500</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L6">
+        <v>500</v>
+      </c>
+      <c r="M6">
+        <v>500</v>
+      </c>
+      <c r="N6">
+        <v>500</v>
+      </c>
+      <c r="O6">
+        <v>500</v>
+      </c>
+      <c r="P6">
+        <v>500</v>
+      </c>
+      <c r="Q6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1278,8 +1411,26 @@
       <c r="K7">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L7">
+        <v>10</v>
+      </c>
+      <c r="M7">
+        <v>10</v>
+      </c>
+      <c r="N7">
+        <v>10</v>
+      </c>
+      <c r="O7">
+        <v>10</v>
+      </c>
+      <c r="P7">
+        <v>10</v>
+      </c>
+      <c r="Q7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1313,8 +1464,26 @@
       <c r="K8">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L8">
+        <v>10</v>
+      </c>
+      <c r="M8">
+        <v>10</v>
+      </c>
+      <c r="N8">
+        <v>10</v>
+      </c>
+      <c r="O8">
+        <v>10</v>
+      </c>
+      <c r="P8">
+        <v>10</v>
+      </c>
+      <c r="Q8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1348,8 +1517,26 @@
       <c r="K9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1383,8 +1570,26 @@
       <c r="K10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1418,8 +1623,26 @@
       <c r="K11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1453,8 +1676,26 @@
       <c r="K12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L12" t="s">
+        <v>12</v>
+      </c>
+      <c r="M12" t="s">
+        <v>12</v>
+      </c>
+      <c r="N12" t="s">
+        <v>12</v>
+      </c>
+      <c r="O12" t="s">
+        <v>12</v>
+      </c>
+      <c r="P12" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1488,8 +1729,26 @@
       <c r="K13">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L13">
+        <v>0.9</v>
+      </c>
+      <c r="M13">
+        <v>0.9</v>
+      </c>
+      <c r="N13">
+        <v>0.9</v>
+      </c>
+      <c r="O13">
+        <v>0.9</v>
+      </c>
+      <c r="P13">
+        <v>0.9</v>
+      </c>
+      <c r="Q13">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1523,8 +1782,26 @@
       <c r="K14">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L14">
+        <v>0.5</v>
+      </c>
+      <c r="M14">
+        <v>0.5</v>
+      </c>
+      <c r="N14">
+        <v>0.5</v>
+      </c>
+      <c r="O14">
+        <v>0.5</v>
+      </c>
+      <c r="P14">
+        <v>0.5</v>
+      </c>
+      <c r="Q14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1558,8 +1835,26 @@
       <c r="K15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1593,8 +1888,26 @@
       <c r="K16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1623,13 +1936,31 @@
         <v>0.1</v>
       </c>
       <c r="J17">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="K17">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0.1</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0.1</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1663,8 +1994,26 @@
       <c r="K18">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L18">
+        <v>0.4</v>
+      </c>
+      <c r="M18">
+        <v>0.4</v>
+      </c>
+      <c r="N18">
+        <v>0.4</v>
+      </c>
+      <c r="O18">
+        <v>0.4</v>
+      </c>
+      <c r="P18">
+        <v>0.4</v>
+      </c>
+      <c r="Q18">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1698,8 +2047,26 @@
       <c r="K19">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L19">
+        <v>0.9</v>
+      </c>
+      <c r="M19">
+        <v>0.9</v>
+      </c>
+      <c r="N19">
+        <v>0.9</v>
+      </c>
+      <c r="O19">
+        <v>0.9</v>
+      </c>
+      <c r="P19">
+        <v>0.9</v>
+      </c>
+      <c r="Q19">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1728,13 +2095,31 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1768,8 +2153,26 @@
       <c r="K21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <v>1</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1803,8 +2206,26 @@
       <c r="K22">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L22">
+        <v>0.9</v>
+      </c>
+      <c r="M22">
+        <v>0.9</v>
+      </c>
+      <c r="N22">
+        <v>0.9</v>
+      </c>
+      <c r="O22">
+        <v>0.9</v>
+      </c>
+      <c r="P22">
+        <v>0.9</v>
+      </c>
+      <c r="Q22">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1838,8 +2259,26 @@
       <c r="K23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1873,8 +2312,26 @@
       <c r="K24">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L24">
+        <v>0.1</v>
+      </c>
+      <c r="M24">
+        <v>0.1</v>
+      </c>
+      <c r="N24">
+        <v>0.1</v>
+      </c>
+      <c r="O24">
+        <v>0.1</v>
+      </c>
+      <c r="P24">
+        <v>0.1</v>
+      </c>
+      <c r="Q24">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1908,8 +2365,26 @@
       <c r="K25">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L25">
+        <v>0.9</v>
+      </c>
+      <c r="M25">
+        <v>0.9</v>
+      </c>
+      <c r="N25">
+        <v>0.9</v>
+      </c>
+      <c r="O25">
+        <v>0.9</v>
+      </c>
+      <c r="P25">
+        <v>0.9</v>
+      </c>
+      <c r="Q25">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1943,8 +2418,26 @@
       <c r="K26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1978,8 +2471,26 @@
       <c r="K27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <v>1</v>
+      </c>
+      <c r="Q27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -2013,8 +2524,26 @@
       <c r="K28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -2048,8 +2577,26 @@
       <c r="K29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <v>1</v>
+      </c>
+      <c r="O29">
+        <v>1</v>
+      </c>
+      <c r="P29">
+        <v>1</v>
+      </c>
+      <c r="Q29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -2078,13 +2625,31 @@
         <v>1E-3</v>
       </c>
       <c r="J30">
-        <v>5.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="K30">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+        <v>1E-3</v>
+      </c>
+      <c r="L30">
+        <v>1E-3</v>
+      </c>
+      <c r="M30">
+        <v>1E-3</v>
+      </c>
+      <c r="N30">
+        <v>1E-3</v>
+      </c>
+      <c r="O30">
+        <v>1E-3</v>
+      </c>
+      <c r="P30">
+        <v>1E-3</v>
+      </c>
+      <c r="Q30">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -2118,8 +2683,26 @@
       <c r="K31">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L31">
+        <v>0.1</v>
+      </c>
+      <c r="M31">
+        <v>0.1</v>
+      </c>
+      <c r="N31">
+        <v>0.1</v>
+      </c>
+      <c r="O31">
+        <v>0.1</v>
+      </c>
+      <c r="P31">
+        <v>0.1</v>
+      </c>
+      <c r="Q31">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -2153,8 +2736,26 @@
       <c r="K32">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L32">
+        <v>2</v>
+      </c>
+      <c r="M32">
+        <v>2</v>
+      </c>
+      <c r="N32">
+        <v>2</v>
+      </c>
+      <c r="O32">
+        <v>2</v>
+      </c>
+      <c r="P32">
+        <v>2</v>
+      </c>
+      <c r="Q32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -2188,8 +2789,26 @@
       <c r="K33">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L33">
+        <v>5</v>
+      </c>
+      <c r="M33">
+        <v>5</v>
+      </c>
+      <c r="N33">
+        <v>5</v>
+      </c>
+      <c r="O33">
+        <v>5</v>
+      </c>
+      <c r="P33">
+        <v>5</v>
+      </c>
+      <c r="Q33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -2223,8 +2842,26 @@
       <c r="K34">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L34">
+        <v>10</v>
+      </c>
+      <c r="M34">
+        <v>10</v>
+      </c>
+      <c r="N34">
+        <v>10</v>
+      </c>
+      <c r="O34">
+        <v>10</v>
+      </c>
+      <c r="P34">
+        <v>10</v>
+      </c>
+      <c r="Q34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -2253,13 +2890,31 @@
         <v>10</v>
       </c>
       <c r="J35">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K35">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+        <v>10</v>
+      </c>
+      <c r="L35">
+        <v>10</v>
+      </c>
+      <c r="M35">
+        <v>10</v>
+      </c>
+      <c r="N35">
+        <v>10</v>
+      </c>
+      <c r="O35">
+        <v>10</v>
+      </c>
+      <c r="P35">
+        <v>10</v>
+      </c>
+      <c r="Q35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -2291,10 +2946,28 @@
         <v>0</v>
       </c>
       <c r="K36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>1</v>
+      </c>
+      <c r="O36">
+        <v>1</v>
+      </c>
+      <c r="P36">
+        <v>1</v>
+      </c>
+      <c r="Q36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -2326,6 +2999,24 @@
         <v>2</v>
       </c>
       <c r="K37">
+        <v>2</v>
+      </c>
+      <c r="L37">
+        <v>2</v>
+      </c>
+      <c r="M37">
+        <v>2</v>
+      </c>
+      <c r="N37">
+        <v>2</v>
+      </c>
+      <c r="O37">
+        <v>2</v>
+      </c>
+      <c r="P37">
+        <v>2</v>
+      </c>
+      <c r="Q37">
         <v>2</v>
       </c>
     </row>

</xml_diff>